<commit_message>
Menambahkan template dan folder yang diperlukan
</commit_message>
<xml_diff>
--- a/templates/template-siswa.xlsx
+++ b/templates/template-siswa.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -428,92 +428,24 @@
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>2024001</v>
+        <v>1234</v>
       </c>
       <c r="B2" t="str">
         <v>1234567890</v>
       </c>
       <c r="C2" t="str">
-        <v>Ahmad Fauzi</v>
+        <v>Nama Siswa</v>
       </c>
       <c r="D2" t="str">
         <v>1</v>
       </c>
       <c r="E2" t="str">
-        <v>L</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="str">
-        <v>2024002</v>
-      </c>
-      <c r="B3" t="str">
-        <v>1234567891</v>
-      </c>
-      <c r="C3" t="str">
-        <v>Siti Nurhaliza</v>
-      </c>
-      <c r="D3" t="str">
-        <v>1</v>
-      </c>
-      <c r="E3" t="str">
-        <v>P</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="str">
-        <v>2024003</v>
-      </c>
-      <c r="B4" t="str">
-        <v>1234567892</v>
-      </c>
-      <c r="C4" t="str">
-        <v>Muhammad Rizki</v>
-      </c>
-      <c r="D4" t="str">
-        <v>2</v>
-      </c>
-      <c r="E4" t="str">
-        <v>L</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="str">
-        <v>2024004</v>
-      </c>
-      <c r="B5" t="str">
-        <v>1234567893</v>
-      </c>
-      <c r="C5" t="str">
-        <v>Putri Rahayu</v>
-      </c>
-      <c r="D5" t="str">
-        <v>2</v>
-      </c>
-      <c r="E5" t="str">
-        <v>P</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="str">
-        <v>2024005</v>
-      </c>
-      <c r="B6" t="str">
-        <v>1234567894</v>
-      </c>
-      <c r="C6" t="str">
-        <v>Budi Santoso</v>
-      </c>
-      <c r="D6" t="str">
-        <v>3</v>
-      </c>
-      <c r="E6" t="str">
         <v>L</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:E6"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E2"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>